<commit_message>
Fechas en las que no trabaja el robot
</commit_message>
<xml_diff>
--- a/Data/Configuración/Config.xlsx
+++ b/Data/Configuración/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ex_nalzate\Documents\Incidencias de Nomina\Configuración\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20DB8317-901C-4E86-92FF-54222D0D807C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBDE036-0091-4727-A927-87C37AB53623}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="122">
   <si>
     <t>Name</t>
   </si>
@@ -372,13 +372,31 @@
   </si>
   <si>
     <t>IMPORTE</t>
+  </si>
+  <si>
+    <t>FileCalendario</t>
+  </si>
+  <si>
+    <t>Calendario.xlsx</t>
+  </si>
+  <si>
+    <t>ColInicio</t>
+  </si>
+  <si>
+    <t>ColFin</t>
+  </si>
+  <si>
+    <t>FECHA INICIO BLOQUEO NOMINA</t>
+  </si>
+  <si>
+    <t>FECHA FIN BLOQUEO NOMINA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -402,16 +420,36 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -419,11 +457,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -434,6 +487,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1859,7 +1918,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2309,9 +2368,30 @@
       </c>
     </row>
     <row r="61" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="62" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="63" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="64" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="62" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A62" t="s">
+        <v>116</v>
+      </c>
+      <c r="B62" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="14.25" customHeight="1" thickBot="1">
+      <c r="A63" t="s">
+        <v>118</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A64" t="s">
+        <v>119</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
     <row r="65" ht="14.25" customHeight="1"/>
     <row r="66" ht="14.25" customHeight="1"/>
     <row r="67" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Final release asignar en vez de cancelar
</commit_message>
<xml_diff>
--- a/Data/Configuración/Config.xlsx
+++ b/Data/Configuración/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ex_nalzate\Documents\Incidencias de Nomina\Configuración\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBDE036-0091-4727-A927-87C37AB53623}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0510E53F-B7FD-456A-8825-AE93220053A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="124">
   <si>
     <t>Name</t>
   </si>
@@ -176,9 +176,6 @@
     <t>SAPCredentials</t>
   </si>
   <si>
-    <t>INNO_SAPCredentials</t>
-  </si>
-  <si>
     <t>FileFallidos</t>
   </si>
   <si>
@@ -269,9 +266,6 @@
     <t>saplogon;EXCEL;OUTLOOK</t>
   </si>
   <si>
-    <t>Sistema Calidad</t>
-  </si>
-  <si>
     <t>ColJob</t>
   </si>
   <si>
@@ -311,9 +305,6 @@
     <t>CorreoResultados</t>
   </si>
   <si>
-    <t>nicolasalzate@chazeypartners.com</t>
-  </si>
-  <si>
     <t>FileConsolidado</t>
   </si>
   <si>
@@ -390,6 +381,21 @@
   </si>
   <si>
     <t>FECHA FIN BLOQUEO NOMINA</t>
+  </si>
+  <si>
+    <t>Sistema productivo</t>
+  </si>
+  <si>
+    <t>CACO_SAPCredentials</t>
+  </si>
+  <si>
+    <t>nicolasalzate@chazeypartners.com;rchinchillam@dospinos.com;torstenschulz@chazeypartners.com</t>
+  </si>
+  <si>
+    <t>UsuarioAsignar</t>
+  </si>
+  <si>
+    <t>diesanchez</t>
   </si>
 </sst>
 </file>
@@ -809,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -857,10 +863,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -881,47 +887,54 @@
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" t="s">
         <v>67</v>
-      </c>
-      <c r="B6" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
         <v>69</v>
-      </c>
-      <c r="B7" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
         <v>79</v>
-      </c>
-      <c r="B8" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" t="s">
+        <v>123</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1917,8 +1930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2062,10 +2075,10 @@
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
         <v>65</v>
-      </c>
-      <c r="B15" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
@@ -2135,34 +2148,34 @@
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
         <v>54</v>
-      </c>
-      <c r="B25" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2171,225 +2184,225 @@
         <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31" t="s">
         <v>58</v>
-      </c>
-      <c r="B31" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32">
         <v>600</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" t="s">
         <v>62</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>63</v>
-      </c>
-      <c r="C33" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" t="s">
         <v>51</v>
-      </c>
-      <c r="B35" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:3" ht="14.25" customHeight="1">
       <c r="A38" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" t="s">
         <v>71</v>
-      </c>
-      <c r="B38" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" t="s">
         <v>73</v>
-      </c>
-      <c r="B40" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1">
       <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" t="s">
         <v>75</v>
-      </c>
-      <c r="B41" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" t="s">
+        <v>93</v>
+      </c>
+      <c r="B48" t="s">
         <v>96</v>
-      </c>
-      <c r="B48" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B50" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="52" spans="1:2" ht="14.25" customHeight="1">
       <c r="A52" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B52" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1">
       <c r="A53" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B53" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="55" spans="1:2" ht="14.25" customHeight="1">
       <c r="A55" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1">
       <c r="A56" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B56" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1">
       <c r="A57" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B57" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="59" spans="1:2" ht="14.25" customHeight="1">
       <c r="A59" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B59" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="14.25" customHeight="1">
       <c r="A60" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B60" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="62" spans="1:2" ht="14.25" customHeight="1">
       <c r="A62" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B62" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="14.25" customHeight="1" thickBot="1">
       <c r="A63" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="14.25" customHeight="1">
       <c r="A64" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Actualización cambio Oracle por SeSuite
</commit_message>
<xml_diff>
--- a/Data/Configuración/Config.xlsx
+++ b/Data/Configuración/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ex_nalzate\Documents\UiPath\DOSPINOS_Incidencias_De_Nomina\Data\Configuración\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ex_nalzate\Documents\Incidencias de Nomina\Configuración\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A394AE27-1B85-4A97-850E-FEDC0D2DB05B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F437634-C144-4675-B489-FC1766D9EEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="136">
   <si>
     <t>Name</t>
   </si>
@@ -263,9 +263,6 @@
     <t>AppsToBeKilled</t>
   </si>
   <si>
-    <t>saplogon;EXCEL;OUTLOOK</t>
-  </si>
-  <si>
     <t>ColJob</t>
   </si>
   <si>
@@ -398,7 +395,43 @@
     <t>diesanchez</t>
   </si>
   <si>
+    <t>saplogon;EXCEL;OUTLOOK;chrome</t>
+  </si>
+  <si>
     <t>FECHA</t>
+  </si>
+  <si>
+    <t>FileFormatoUnitario</t>
+  </si>
+  <si>
+    <t>Formato unitario.xlsx</t>
+  </si>
+  <si>
+    <t>SheetTemplateU</t>
+  </si>
+  <si>
+    <t>OracleCredentials</t>
+  </si>
+  <si>
+    <t>INNO_OracleCredentials</t>
+  </si>
+  <si>
+    <t>URLOracle</t>
+  </si>
+  <si>
+    <t>https://fa-enfw-test-saasfaprod1.fa.ocs.oraclecloud.com/</t>
+  </si>
+  <si>
+    <t>OracleCategory</t>
+  </si>
+  <si>
+    <t>Envío incidencias nómina</t>
+  </si>
+  <si>
+    <t>OracleAsignado</t>
+  </si>
+  <si>
+    <t>DIEGO ARMANDO SANCHEZ</t>
   </si>
 </sst>
 </file>
@@ -444,7 +477,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -454,6 +487,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -485,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -502,6 +541,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -819,15 +859,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.77734375" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -876,7 +916,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="28.8">
+    <row r="4" spans="1:26" ht="30">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -909,33 +949,33 @@
         <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" t="s">
         <v>122</v>
-      </c>
-      <c r="B13" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1933,16 +1973,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.33203125" customWidth="1"/>
-    <col min="4" max="26" width="8.77734375" customWidth="1"/>
+    <col min="3" max="3" width="75.28515625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1979,7 +2019,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2159,26 +2199,26 @@
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" t="s">
         <v>84</v>
-      </c>
-      <c r="B26" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" t="s">
         <v>88</v>
-      </c>
-      <c r="B27" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2187,7 +2227,7 @@
         <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
@@ -2195,7 +2235,7 @@
         <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C31" t="s">
         <v>58</v>
@@ -2237,7 +2277,7 @@
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2276,58 +2316,58 @@
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" t="s">
         <v>80</v>
-      </c>
-      <c r="B43" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" t="s">
         <v>82</v>
-      </c>
-      <c r="B45" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" t="s">
         <v>86</v>
-      </c>
-      <c r="B46" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1">
       <c r="A49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1">
       <c r="A50" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" t="s">
         <v>97</v>
-      </c>
-      <c r="B50" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="52" spans="1:2" ht="14.25" customHeight="1">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B52" t="s">
         <v>124</v>
@@ -2335,95 +2375,137 @@
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1">
       <c r="A53" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" t="s">
         <v>101</v>
-      </c>
-      <c r="B53" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="55" spans="1:2" ht="14.25" customHeight="1">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1">
       <c r="A56" t="s">
+        <v>104</v>
+      </c>
+      <c r="B56" t="s">
         <v>105</v>
-      </c>
-      <c r="B56" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="14.25" customHeight="1">
       <c r="A57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B57" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="59" spans="1:2" ht="14.25" customHeight="1">
       <c r="A59" t="s">
+        <v>108</v>
+      </c>
+      <c r="B59" t="s">
         <v>109</v>
-      </c>
-      <c r="B59" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="14.25" customHeight="1">
       <c r="A60" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" t="s">
         <v>111</v>
-      </c>
-      <c r="B60" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="62" spans="1:2" ht="14.25" customHeight="1">
       <c r="A62" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" t="s">
         <v>113</v>
-      </c>
-      <c r="B62" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="14.25" customHeight="1" thickBot="1">
       <c r="A63" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="14.25" customHeight="1">
       <c r="A64" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="66" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A66" t="s">
+        <v>125</v>
+      </c>
+      <c r="B66" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A67" t="s">
+        <v>127</v>
+      </c>
+      <c r="B67" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="69" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A69" t="s">
+        <v>128</v>
+      </c>
+      <c r="B69" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A70" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A71" t="s">
+        <v>132</v>
+      </c>
+      <c r="B71" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A72" t="s">
+        <v>134</v>
+      </c>
+      <c r="B72" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="74" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="75" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="76" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="77" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="78" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="79" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="80" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="81" ht="14.25" customHeight="1"/>
     <row r="82" ht="14.25" customHeight="1"/>
     <row r="83" ht="14.25" customHeight="1"/>
@@ -3351,12 +3433,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.77734375" customWidth="1"/>
-    <col min="2" max="2" width="30.21875" customWidth="1"/>
-    <col min="3" max="3" width="60.21875" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>